<commit_message>
Add 12 new GitHub repositories from Risk Tools list
Downloaded additional risk assessment tools across multiple categories:
- Environment: CodeCarbon
- Technical: RAGAS, DeepEval, PromptFoo
- Trust: LIME, Captum
- Fundamental Rights: Fairlearn, Aequitas
- Societal: Detoxify
- Third-Party: ScanCode Toolkit
- Health & Safety: Uncertainty Toolbox
- EU AI Act Compliance: TheHive

Total repositories now: 35 across all risk categories
Added download_from_list.py automation script and updated documentation

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Risk_Assessment_Guide.xlsx
+++ b/AI_Risk_Assessment_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miachen/Desktop/Mia/DT Master/Tech/Hackthon/geminihackathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF73E99-26B6-164C-85E3-4E1E77D5E04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135C3469-3049-A14F-A9DF-347F966F5165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="500" windowWidth="33600" windowHeight="19580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -5998,10 +5998,6 @@
     <xf numFmtId="0" fontId="13" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6017,6 +6013,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6333,12 +6333,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6475,8 +6475,8 @@
     <col min="4" max="4" width="25" style="33" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="50" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="46" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
     <col min="10" max="10" width="40" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
@@ -6501,10 +6501,10 @@
       <c r="F1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="42" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="34" t="s">
@@ -6528,16 +6528,16 @@
       <c r="D2" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="43" t="s">
         <v>74</v>
       </c>
       <c r="F2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I2" s="27" t="s">
@@ -6567,10 +6567,10 @@
       <c r="F3" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="27" t="s">
@@ -6600,10 +6600,10 @@
       <c r="F4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="48" t="s">
+      <c r="G4" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="27" t="s">
@@ -6633,10 +6633,10 @@
       <c r="F5" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="27" t="s">
@@ -6666,10 +6666,10 @@
       <c r="F6" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="27" t="s">
@@ -6699,10 +6699,10 @@
       <c r="F7" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="27" t="s">
@@ -6732,10 +6732,10 @@
       <c r="F8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="27" t="s">
@@ -6765,10 +6765,10 @@
       <c r="F9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="48" t="s">
+      <c r="G9" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="27" t="s">
@@ -6798,10 +6798,10 @@
       <c r="F10" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G10" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="48" t="s">
+      <c r="G10" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="27" t="s">
@@ -6831,10 +6831,10 @@
       <c r="F11" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="27" t="s">
@@ -6864,10 +6864,10 @@
       <c r="F12" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G12" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="48" t="s">
+      <c r="G12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="27" t="s">
@@ -6897,10 +6897,10 @@
       <c r="F13" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="G13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="27" t="s">
@@ -6930,10 +6930,10 @@
       <c r="F14" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="G14" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="48" t="s">
+      <c r="G14" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="27" t="s">
@@ -6963,10 +6963,10 @@
       <c r="F15" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="G15" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="48" t="s">
+      <c r="G15" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="27" t="s">
@@ -6996,10 +6996,10 @@
       <c r="F16" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="48" t="s">
+      <c r="G16" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="27" t="s">
@@ -7029,10 +7029,10 @@
       <c r="F17" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="G17" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="27" t="s">
@@ -7062,10 +7062,10 @@
       <c r="F18" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="48" t="s">
+      <c r="H18" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="27" t="s">
@@ -7095,10 +7095,10 @@
       <c r="F19" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="27" t="s">
@@ -7128,10 +7128,10 @@
       <c r="F20" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="48" t="s">
+      <c r="H20" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="27" t="s">
@@ -7161,10 +7161,10 @@
       <c r="F21" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="48" t="s">
+      <c r="H21" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="27" t="s">
@@ -7194,10 +7194,10 @@
       <c r="F22" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="G22" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="48" t="s">
+      <c r="G22" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="27" t="s">
@@ -7227,10 +7227,10 @@
       <c r="F23" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="G23" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="48" t="s">
+      <c r="G23" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="27" t="s">
@@ -7245,7 +7245,7 @@
     </row>
     <row r="24" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="28"/>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="45" t="s">
         <v>1871</v>
       </c>
       <c r="C24" s="31" t="s">
@@ -7260,10 +7260,10 @@
       <c r="F24" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="48" t="s">
+      <c r="G24" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="27" t="s">
@@ -7293,10 +7293,10 @@
       <c r="F25" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="G25" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="48" t="s">
+      <c r="G25" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="27" t="s">
@@ -7326,10 +7326,10 @@
       <c r="F26" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="48" t="s">
+      <c r="H26" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="27" t="s">
@@ -7359,10 +7359,10 @@
       <c r="F27" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="27" t="s">
@@ -7392,10 +7392,10 @@
       <c r="F28" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="G28" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="48" t="s">
+      <c r="H28" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I28" s="27" t="s">
@@ -7425,10 +7425,10 @@
       <c r="F29" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="48" t="s">
+      <c r="G29" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="27" t="s">
@@ -7458,10 +7458,10 @@
       <c r="F30" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="48" t="s">
+      <c r="G30" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I30" s="27" t="s">
@@ -7491,10 +7491,10 @@
       <c r="F31" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="48" t="s">
+      <c r="G31" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I31" s="27" t="s">
@@ -7524,10 +7524,10 @@
       <c r="F32" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="G32" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="48" t="s">
+      <c r="G32" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I32" s="27" t="s">
@@ -7557,10 +7557,10 @@
       <c r="F33" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" s="48" t="s">
+      <c r="G33" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I33" s="27" t="s">
@@ -7590,10 +7590,10 @@
       <c r="F34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="48" t="s">
+      <c r="G34" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="48" t="s">
+      <c r="H34" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I34" s="27" t="s">
@@ -7623,10 +7623,10 @@
       <c r="F35" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G35" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="48" t="s">
+      <c r="G35" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I35" s="27" t="s">
@@ -7656,10 +7656,10 @@
       <c r="F36" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="G36" s="48" t="s">
+      <c r="G36" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I36" s="27" t="s">
@@ -7689,10 +7689,10 @@
       <c r="F37" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G37" s="48" t="s">
+      <c r="G37" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="48" t="s">
+      <c r="H37" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I37" s="27" t="s">
@@ -7722,10 +7722,10 @@
       <c r="F38" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="48" t="s">
+      <c r="G38" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H38" s="48" t="s">
+      <c r="H38" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I38" s="27" t="s">
@@ -7755,10 +7755,10 @@
       <c r="F39" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="48" t="s">
+      <c r="G39" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="48" t="s">
+      <c r="H39" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I39" s="27" t="s">
@@ -7788,10 +7788,10 @@
       <c r="F40" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="G40" s="48" t="s">
+      <c r="G40" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="48" t="s">
+      <c r="H40" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I40" s="27" t="s">
@@ -7821,10 +7821,10 @@
       <c r="F41" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="G41" s="48" t="s">
+      <c r="G41" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="48" t="s">
+      <c r="H41" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I41" s="27" t="s">
@@ -7854,10 +7854,10 @@
       <c r="F42" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="G42" s="48" t="s">
+      <c r="G42" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="44" t="s">
         <v>12</v>
       </c>
       <c r="I42" s="27" t="s">
@@ -7887,10 +7887,10 @@
       <c r="F43" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="G43" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="48" t="s">
+      <c r="G43" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I43" s="27" t="s">
@@ -7920,10 +7920,10 @@
       <c r="F44" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="48" t="s">
+      <c r="H44" s="44" t="s">
         <v>23</v>
       </c>
       <c r="I44" s="27" t="s">
@@ -8023,7 +8023,7 @@
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="49" t="s">
+      <c r="B60" s="45" t="s">
         <v>1871</v>
       </c>
       <c r="C60" s="31">
@@ -8043,20 +8043,20 @@
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="35" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="35" customWidth="1"/>
     <col min="10" max="10" width="57.83203125" customWidth="1"/>
     <col min="11" max="11" width="117" customWidth="1"/>
     <col min="12" max="12" width="73.33203125" bestFit="1" customWidth="1"/>
@@ -8124,7 +8124,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="17" customFormat="1" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>289</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -10345,7 +10345,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>566</v>
       </c>
@@ -10734,7 +10734,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>617</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>691</v>
       </c>
@@ -11320,7 +11320,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="78" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="23" t="s">
         <v>739</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="81" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="23" t="s">
         <v>739</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="86" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
         <v>739</v>
       </c>
@@ -12518,8 +12518,8 @@
     <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="F106" s="19"/>
       <c r="G106" s="20"/>
-      <c r="H106" s="43"/>
-      <c r="I106" s="44"/>
+      <c r="H106" s="48"/>
+      <c r="I106" s="49"/>
       <c r="J106" s="20"/>
       <c r="K106" s="19"/>
     </row>
@@ -12529,8 +12529,8 @@
       </c>
       <c r="F107" s="19"/>
       <c r="G107" s="20"/>
-      <c r="H107" s="43"/>
-      <c r="I107" s="43"/>
+      <c r="H107" s="48"/>
+      <c r="I107" s="48"/>
     </row>
     <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -12541,8 +12541,8 @@
       </c>
       <c r="F108" s="19"/>
       <c r="G108" s="20"/>
-      <c r="H108" s="43"/>
-      <c r="I108" s="43"/>
+      <c r="H108" s="48"/>
+      <c r="I108" s="48"/>
       <c r="K108" s="20"/>
     </row>
     <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
@@ -12554,8 +12554,8 @@
       </c>
       <c r="F109" s="19"/>
       <c r="G109" s="20"/>
-      <c r="H109" s="43"/>
-      <c r="I109" s="44"/>
+      <c r="H109" s="48"/>
+      <c r="I109" s="49"/>
       <c r="J109" s="20"/>
       <c r="K109" s="19"/>
     </row>
@@ -12568,8 +12568,8 @@
       </c>
       <c r="F110" s="19"/>
       <c r="G110" s="20"/>
-      <c r="H110" s="43"/>
-      <c r="I110" s="43"/>
+      <c r="H110" s="48"/>
+      <c r="I110" s="48"/>
     </row>
     <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -12580,8 +12580,8 @@
       </c>
       <c r="F111" s="19"/>
       <c r="G111" s="20"/>
-      <c r="H111" s="43"/>
-      <c r="I111" s="43"/>
+      <c r="H111" s="48"/>
+      <c r="I111" s="48"/>
       <c r="K111" s="20"/>
     </row>
     <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
@@ -12593,8 +12593,8 @@
       </c>
       <c r="F112" s="19"/>
       <c r="G112" s="20"/>
-      <c r="H112" s="43"/>
-      <c r="I112" s="44"/>
+      <c r="H112" s="48"/>
+      <c r="I112" s="49"/>
       <c r="J112" s="20"/>
       <c r="K112" s="19"/>
     </row>
@@ -12607,8 +12607,8 @@
       </c>
       <c r="F113" s="19"/>
       <c r="G113" s="20"/>
-      <c r="H113" s="43"/>
-      <c r="I113" s="43"/>
+      <c r="H113" s="48"/>
+      <c r="I113" s="48"/>
     </row>
     <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
@@ -12617,8 +12617,8 @@
       <c r="C114" t="s">
         <v>902</v>
       </c>
-      <c r="H114" s="43"/>
-      <c r="I114" s="43"/>
+      <c r="H114" s="48"/>
+      <c r="I114" s="48"/>
       <c r="K114" s="20"/>
     </row>
     <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
@@ -12628,118 +12628,104 @@
       <c r="C115" t="s">
         <v>902</v>
       </c>
-      <c r="H115" s="43"/>
-      <c r="I115" s="44"/>
+      <c r="H115" s="48"/>
+      <c r="I115" s="49"/>
       <c r="J115" s="20"/>
       <c r="K115" s="19"/>
     </row>
     <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H116" s="43"/>
-      <c r="I116" s="43"/>
+      <c r="H116" s="48"/>
+      <c r="I116" s="48"/>
     </row>
     <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H117" s="43"/>
-      <c r="I117" s="43"/>
+      <c r="H117" s="48"/>
+      <c r="I117" s="48"/>
       <c r="K117" s="20"/>
     </row>
     <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H118" s="43"/>
-      <c r="I118" s="44"/>
+      <c r="H118" s="48"/>
+      <c r="I118" s="49"/>
       <c r="J118" s="20"/>
       <c r="K118" s="19"/>
     </row>
     <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H119" s="43"/>
-      <c r="I119" s="43"/>
+      <c r="H119" s="48"/>
+      <c r="I119" s="48"/>
     </row>
     <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H120" s="43"/>
-      <c r="I120" s="43"/>
+      <c r="H120" s="48"/>
+      <c r="I120" s="48"/>
       <c r="K120" s="20"/>
     </row>
     <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H121" s="43"/>
-      <c r="I121" s="44"/>
+      <c r="H121" s="48"/>
+      <c r="I121" s="49"/>
       <c r="J121" s="20"/>
       <c r="K121" s="19"/>
     </row>
     <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H122" s="43"/>
-      <c r="I122" s="43"/>
+      <c r="H122" s="48"/>
+      <c r="I122" s="48"/>
     </row>
     <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H123" s="43"/>
-      <c r="I123" s="43"/>
+      <c r="H123" s="48"/>
+      <c r="I123" s="48"/>
       <c r="K123" s="20"/>
     </row>
     <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H124" s="43"/>
-      <c r="I124" s="44"/>
+      <c r="H124" s="48"/>
+      <c r="I124" s="49"/>
       <c r="J124" s="20"/>
       <c r="K124" s="19"/>
     </row>
     <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H125" s="43"/>
-      <c r="I125" s="43"/>
+      <c r="H125" s="48"/>
+      <c r="I125" s="48"/>
     </row>
     <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H126" s="43"/>
-      <c r="I126" s="43"/>
+      <c r="H126" s="48"/>
+      <c r="I126" s="48"/>
       <c r="K126" s="20"/>
     </row>
     <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H127" s="43"/>
-      <c r="I127" s="44"/>
+      <c r="H127" s="48"/>
+      <c r="I127" s="49"/>
       <c r="J127" s="20"/>
       <c r="K127" s="19"/>
     </row>
     <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H128" s="43"/>
-      <c r="I128" s="43"/>
+      <c r="H128" s="48"/>
+      <c r="I128" s="48"/>
     </row>
     <row r="129" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H129" s="43"/>
-      <c r="I129" s="43"/>
+      <c r="H129" s="48"/>
+      <c r="I129" s="48"/>
       <c r="K129" s="20"/>
     </row>
     <row r="130" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H130" s="43"/>
-      <c r="I130" s="44"/>
+      <c r="H130" s="48"/>
+      <c r="I130" s="49"/>
       <c r="J130" s="20"/>
       <c r="K130" s="19"/>
     </row>
     <row r="131" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H131" s="43"/>
-      <c r="I131" s="43"/>
+      <c r="H131" s="48"/>
+      <c r="I131" s="48"/>
     </row>
     <row r="132" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="H132" s="43"/>
-      <c r="I132" s="43"/>
+      <c r="H132" s="48"/>
+      <c r="I132" s="48"/>
       <c r="K132" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R132" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Business"/>
-        <filter val="EU AI Act Compliance"/>
-        <filter val="Health &amp; Safety"/>
-        <filter val="Legal"/>
-        <filter val="Societal"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="12">
-      <filters>
-        <filter val="No"/>
-      </filters>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="18">
-    <mergeCell ref="H124:H126"/>
-    <mergeCell ref="I124:I126"/>
-    <mergeCell ref="H106:H108"/>
-    <mergeCell ref="H121:H123"/>
-    <mergeCell ref="I106:I108"/>
     <mergeCell ref="I130:I132"/>
     <mergeCell ref="H118:H120"/>
     <mergeCell ref="I118:I120"/>
@@ -12753,6 +12739,11 @@
     <mergeCell ref="H127:H129"/>
     <mergeCell ref="I127:I129"/>
     <mergeCell ref="H115:H117"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="I124:I126"/>
+    <mergeCell ref="H106:H108"/>
+    <mergeCell ref="H121:H123"/>
+    <mergeCell ref="I106:I108"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -15496,14 +15487,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>1212</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -15828,14 +15819,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>1284</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -16139,14 +16130,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>1343</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">

</xml_diff>